<commit_message>
Pre visualizar receitas adicionado
Pre visualizar receitas adicionado
</commit_message>
<xml_diff>
--- a/Especificacao/especificacaoUseCases.xlsx
+++ b/Especificacao/especificacaoUseCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\35192\Desktop\Universidade\MyChef\Especificacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjsf3\Desktop\MIEI\LI4\MyChef\Especificacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A193D082-FB79-45BF-A4DD-952C42231AEF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1303021D-E578-431F-9143-520C9B977E05}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="2076" windowWidth="17280" windowHeight="8964" firstSheet="3" activeTab="4" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="4" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Fazer Autenticação" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
   <si>
     <t>Actor input</t>
   </si>
@@ -189,6 +189,42 @@
   </si>
   <si>
     <t>Pré-visualizar receitas</t>
+  </si>
+  <si>
+    <t>Vê lista de receita</t>
+  </si>
+  <si>
+    <t>2. Apresenta lista de receitas</t>
+  </si>
+  <si>
+    <t>Cenário alternativo 1[Seleciona Ingredientes que não pretende confecionar ](passo 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1 Indica quais os ingredientes
+que não pretende utilizar </t>
+  </si>
+  <si>
+    <t>Regressa a 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1 Indica quais os ingredientes
+que pretende utilizar </t>
+  </si>
+  <si>
+    <t>Cenário alternativo   2[Indica ingredientes que pretende utilizar](passo 1)</t>
+  </si>
+  <si>
+    <t>2.1Indica que não conseguiu encontrar 
+pratos para a especificaçao feita pelo
+utlizador</t>
+  </si>
+  <si>
+    <t>Exceção 1
+[Não encontra lista de pratos para a especificaçao acima
+(passo 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleciona tipo de prato a confecionar </t>
   </si>
 </sst>
 </file>
@@ -225,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -470,11 +506,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -493,27 +580,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -527,15 +593,76 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,57 +979,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
   <dimension ref="B1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="B2:D19"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="16.19921875" customWidth="1"/>
-    <col min="3" max="3" width="33.296875" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D2" s="22"/>
+    </row>
+    <row r="3" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="16"/>
-    </row>
-    <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="17" t="s">
+      <c r="D5" s="24"/>
+    </row>
+    <row r="6" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="25" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -912,62 +1039,62 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="18"/>
+    <row r="7" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="26"/>
       <c r="C7" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="18"/>
+    <row r="8" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="26"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="18"/>
+    <row r="9" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="26"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="18"/>
+    <row r="10" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="26"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="18"/>
+    <row r="11" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="26"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="18"/>
+    <row r="12" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="26"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="18"/>
+    <row r="13" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="26"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="18"/>
+    <row r="14" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="26"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="18"/>
+    <row r="15" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="26"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="18"/>
+    <row r="16" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="26"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="12" t="s">
+    <row r="17" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="4"/>
@@ -975,13 +1102,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="12"/>
+    <row r="18" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B18" s="20"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="12"/>
+    <row r="19" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="20"/>
       <c r="C19" s="6"/>
       <c r="D19" s="11"/>
     </row>
@@ -1002,57 +1129,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5665B78-CE62-4C13-BA3D-9BD966D01A4F}">
   <dimension ref="B1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" workbookViewId="0">
+    <sheetView topLeftCell="B13" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="16.19921875" customWidth="1"/>
-    <col min="3" max="3" width="33.296875" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D2" s="22"/>
+    </row>
+    <row r="3" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="16"/>
-    </row>
-    <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="17" t="s">
+      <c r="D5" s="24"/>
+    </row>
+    <row r="6" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="25" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1062,109 +1189,109 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="18"/>
+    <row r="7" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="26"/>
       <c r="C7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="18"/>
+    <row r="8" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="26"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="18"/>
+    <row r="9" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="26"/>
       <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="18"/>
+    <row r="10" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="26"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="18"/>
+    <row r="11" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="26"/>
       <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="18"/>
+    <row r="12" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="26"/>
       <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="18"/>
+    <row r="13" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="26"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="18"/>
+    <row r="14" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="26"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="18"/>
+    <row r="15" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="26"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="18"/>
+    <row r="16" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="26"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="12" t="s">
+    <row r="17" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="20" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="12"/>
+    <row r="18" spans="2:4" ht="24.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B18" s="20"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="12"/>
+    <row r="19" spans="2:4" ht="49.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="20"/>
       <c r="C19" s="6"/>
       <c r="D19" s="11"/>
     </row>
-    <row r="20" spans="2:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="12" t="s">
+    <row r="20" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B20" s="20" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="12"/>
+    <row r="21" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B21" s="20"/>
       <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="12"/>
+    <row r="22" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B22" s="20"/>
       <c r="C22" s="6"/>
       <c r="D22" s="11"/>
     </row>
@@ -1186,143 +1313,143 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054B29E9-D1D3-435F-ADF1-FE65B0763CC2}">
   <dimension ref="B1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B8" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="16.19921875" customWidth="1"/>
-    <col min="3" max="3" width="33.296875" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D2" s="22"/>
+    </row>
+    <row r="3" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="16"/>
-    </row>
-    <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="24" t="s">
+      <c r="D5" s="24"/>
+    </row>
+    <row r="6" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="14" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="25"/>
-      <c r="C7" s="22" t="s">
+    <row r="7" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="28"/>
+      <c r="C7" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="25"/>
-      <c r="C8" s="23"/>
+    <row r="8" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="28"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="25"/>
-      <c r="C9" s="23" t="s">
+    <row r="9" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="28"/>
+      <c r="C9" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="25"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="20" t="s">
+    <row r="10" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="28"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="25"/>
-      <c r="C11" s="23"/>
+    <row r="11" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="28"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="25"/>
-      <c r="C12" s="23" t="s">
+    <row r="12" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="28"/>
+      <c r="C12" s="16" t="s">
         <v>44</v>
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="25"/>
-      <c r="C13" s="23"/>
+    <row r="13" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="28"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="25"/>
-      <c r="C14" s="23"/>
+    <row r="14" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="28"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="25"/>
-      <c r="C15" s="23" t="s">
+    <row r="15" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="28"/>
+      <c r="C15" s="16" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="25"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="20" t="s">
+    <row r="16" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="28"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="25"/>
-      <c r="C17" s="26"/>
+    <row r="17" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="28"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="12" t="s">
+    <row r="18" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B18" s="20" t="s">
         <v>45</v>
       </c>
       <c r="C18" s="5"/>
@@ -1330,24 +1457,24 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="12"/>
+    <row r="19" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="20"/>
       <c r="C19" s="5"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="12"/>
+    <row r="20" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B20" s="20"/>
       <c r="C20" s="6"/>
       <c r="D20" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B18:B20"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="B6:B17"/>
-    <mergeCell ref="B18:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1357,125 +1484,125 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B982C2AA-2A13-4FE1-A2EE-7FEF12C78847}">
   <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="16.19921875" customWidth="1"/>
-    <col min="3" max="3" width="33.296875" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D2" s="22"/>
+    </row>
+    <row r="3" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="16"/>
-    </row>
-    <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="24" t="s">
+      <c r="D5" s="24"/>
+    </row>
+    <row r="6" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="14" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="25"/>
-      <c r="C7" s="22" t="s">
+    <row r="7" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="28"/>
+      <c r="C7" s="15" t="s">
         <v>49</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="25"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="20" t="s">
+    <row r="8" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="28"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="25"/>
-      <c r="C9" s="23" t="s">
+    <row r="9" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="28"/>
+      <c r="C9" s="16" t="s">
         <v>51</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="25"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="20"/>
-    </row>
-    <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="25"/>
-      <c r="C11" s="23"/>
+    <row r="10" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="28"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="28"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="25"/>
-      <c r="C12" s="23"/>
+    <row r="12" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="28"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="25"/>
-      <c r="C13" s="23"/>
+    <row r="13" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="28"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="25"/>
-      <c r="C14" s="23"/>
+    <row r="14" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="28"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="25"/>
-      <c r="C15" s="23"/>
+    <row r="15" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="28"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="25"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="20"/>
-    </row>
-    <row r="17" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="25"/>
-      <c r="C17" s="28"/>
+    <row r="16" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="28"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="28"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="3"/>
     </row>
   </sheetData>
@@ -1495,145 +1622,162 @@
   <dimension ref="B1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="16.19921875" customWidth="1"/>
-    <col min="3" max="3" width="33.296875" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D2" s="22"/>
+    </row>
+    <row r="3" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="16"/>
-    </row>
-    <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="24" t="s">
+      <c r="C5" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="24"/>
+    </row>
+    <row r="6" spans="2:4" ht="19" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="14" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="25"/>
-      <c r="C7" s="22"/>
+    <row r="7" spans="2:4" ht="37" x14ac:dyDescent="0.45">
+      <c r="B7" s="30"/>
+      <c r="C7" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="25"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="25"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="25"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="20"/>
-    </row>
-    <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="25"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="25"/>
-      <c r="C12" s="23"/>
+    <row r="8" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="31"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="78.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="34"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="32"/>
+    </row>
+    <row r="11" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="40"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="25"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="25"/>
-      <c r="C14" s="23"/>
+    <row r="13" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="20"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="20"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="25"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="25"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="20"/>
-    </row>
-    <row r="17" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="25"/>
-      <c r="C17" s="26"/>
+    <row r="15" spans="2:4" ht="53" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B16" s="36"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="39"/>
+    </row>
+    <row r="17" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="37"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="12"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="12"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="11"/>
+    <row r="18" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="D18" s="38"/>
+    </row>
+    <row r="19" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+    </row>
+    <row r="20" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B11"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B17"/>
-    <mergeCell ref="B18:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
use cases e maquina de estado
</commit_message>
<xml_diff>
--- a/Especificacao/especificacaoUseCases.xlsx
+++ b/Especificacao/especificacaoUseCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjsf3\Desktop\MIEI\LI4\MyChef\Especificacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joao/Desktop/Desktop_iCloud/Universidade/3ºano/2ºsemestre/LI4/MyChef/Especificacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1303021D-E578-431F-9143-520C9B977E05}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27B9C4F-48BA-AD4B-A225-BAC792FA04C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="4" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Fazer Autenticação" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Preparar Receita" sheetId="4" r:id="rId3"/>
     <sheet name="Selecionar Receita" sheetId="5" r:id="rId4"/>
     <sheet name="Pré-visualizar receitas" sheetId="6" r:id="rId5"/>
+    <sheet name="Folha1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
   <si>
     <t>Actor input</t>
   </si>
@@ -176,62 +177,70 @@
     <t>Selecionar Receita</t>
   </si>
   <si>
-    <t>Receita escolhida</t>
-  </si>
-  <si>
-    <t>1. Indica uma receita</t>
-  </si>
-  <si>
-    <t>2. Apresenta todos os dados necessários sobre a receita</t>
-  </si>
-  <si>
-    <t>3.Confirma escolha da receita</t>
-  </si>
-  <si>
     <t>Pré-visualizar receitas</t>
   </si>
   <si>
-    <t>Vê lista de receita</t>
-  </si>
-  <si>
     <t>2. Apresenta lista de receitas</t>
   </si>
   <si>
-    <t>Cenário alternativo 1[Seleciona Ingredientes que não pretende confecionar ](passo 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1 Indica quais os ingredientes
-que não pretende utilizar </t>
-  </si>
-  <si>
-    <t>Regressa a 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1 Indica quais os ingredientes
-que pretende utilizar </t>
-  </si>
-  <si>
-    <t>Cenário alternativo   2[Indica ingredientes que pretende utilizar](passo 1)</t>
-  </si>
-  <si>
-    <t>2.1Indica que não conseguiu encontrar 
-pratos para a especificaçao feita pelo
-utlizador</t>
+    <t>Lista de receitas disponibilizadas</t>
+  </si>
+  <si>
+    <t>1. Solicita lista de receitas</t>
+  </si>
+  <si>
+    <t>Filtrar Receitas</t>
+  </si>
+  <si>
+    <t>1. &lt;&lt;include&gt;&gt; Pré-visualizar Receitas</t>
+  </si>
+  <si>
+    <t>2. Apresenta filtros pré-definidos</t>
+  </si>
+  <si>
+    <t>3. Seleciona filtros pretendidos</t>
+  </si>
+  <si>
+    <t>4. Procura receitas  na base de dados.</t>
+  </si>
+  <si>
+    <t>5. Apresenta nova lista de receitas consoante os filtros selecionados</t>
   </si>
   <si>
     <t>Exceção 1
-[Não encontra lista de pratos para a especificaçao acima
-(passo 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Seleciona tipo de prato a confecionar </t>
+[Não encontra receitas para a filtragem pretendida]
+(passo 4)</t>
+  </si>
+  <si>
+    <t>4.1. Indica que não existem receitas disponíveis.</t>
+  </si>
+  <si>
+    <t>1.&lt;&lt;include&gt;&gt; Pré-visualizar Receitas</t>
+  </si>
+  <si>
+    <t>2. Seleciona Receita</t>
+  </si>
+  <si>
+    <t>3. Apresenta dados da receita</t>
+  </si>
+  <si>
+    <t>Receita confirmada</t>
+  </si>
+  <si>
+    <t>4. Confirma Receita</t>
+  </si>
+  <si>
+    <t>4.1. Retorna à janela de pré-visualização</t>
+  </si>
+  <si>
+    <t>Exceção 1 [Não confirma Receita](passo 4)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -245,6 +254,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri (corpo)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -494,64 +508,76 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -595,10 +621,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -623,46 +652,39 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -983,7 +1005,7 @@
       <selection activeCell="B17" sqref="B17:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
@@ -991,45 +1013,45 @@
     <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:4" ht="17" thickBot="1"/>
+    <row r="2" spans="2:4" ht="20" thickBot="1">
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="22"/>
-    </row>
-    <row r="3" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="2:4" ht="20" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="22"/>
-    </row>
-    <row r="4" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="2:4" ht="20" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="22"/>
-    </row>
-    <row r="5" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="24"/>
-    </row>
-    <row r="6" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="25" t="s">
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1">
+      <c r="B6" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1039,62 +1061,62 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="26"/>
+    <row r="7" spans="2:4" ht="41" thickBot="1">
+      <c r="B7" s="27"/>
       <c r="C7" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="26"/>
+    <row r="8" spans="2:4" ht="20" thickBot="1">
+      <c r="B8" s="27"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="26"/>
+    <row r="9" spans="2:4" ht="20" thickBot="1">
+      <c r="B9" s="27"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="26"/>
+    <row r="10" spans="2:4" ht="20" thickBot="1">
+      <c r="B10" s="27"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="26"/>
+    <row r="11" spans="2:4" ht="20" thickBot="1">
+      <c r="B11" s="27"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="26"/>
+    <row r="12" spans="2:4" ht="20" thickBot="1">
+      <c r="B12" s="27"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="26"/>
+    <row r="13" spans="2:4" ht="20" thickBot="1">
+      <c r="B13" s="27"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="26"/>
+    <row r="14" spans="2:4" ht="20" thickBot="1">
+      <c r="B14" s="27"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="26"/>
+    <row r="15" spans="2:4" ht="20" thickBot="1">
+      <c r="B15" s="27"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="26"/>
+    <row r="16" spans="2:4" ht="20" thickBot="1">
+      <c r="B16" s="27"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="20" t="s">
+    <row r="17" spans="2:4" ht="20" thickBot="1">
+      <c r="B17" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="4"/>
@@ -1102,13 +1124,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="20"/>
+    <row r="18" spans="2:4" ht="20" thickBot="1">
+      <c r="B18" s="21"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="20"/>
+    <row r="19" spans="2:4" ht="20" thickBot="1">
+      <c r="B19" s="21"/>
       <c r="C19" s="6"/>
       <c r="D19" s="11"/>
     </row>
@@ -1133,7 +1155,7 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
@@ -1141,45 +1163,45 @@
     <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:4" ht="17" thickBot="1"/>
+    <row r="2" spans="2:4" ht="20" thickBot="1">
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="22"/>
-    </row>
-    <row r="3" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="2:4" ht="20" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="22"/>
-    </row>
-    <row r="4" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="2:4" ht="20" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="22"/>
-    </row>
-    <row r="5" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="24"/>
-    </row>
-    <row r="6" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="25" t="s">
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1">
+      <c r="B6" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1189,72 +1211,72 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="26"/>
+    <row r="7" spans="2:4" ht="21" thickBot="1">
+      <c r="B7" s="27"/>
       <c r="C7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="26"/>
+    <row r="8" spans="2:4" ht="20" thickBot="1">
+      <c r="B8" s="27"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="26"/>
+    <row r="9" spans="2:4" ht="20" thickBot="1">
+      <c r="B9" s="27"/>
       <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="26"/>
+    <row r="10" spans="2:4" ht="20" thickBot="1">
+      <c r="B10" s="27"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="26"/>
+    <row r="11" spans="2:4" ht="20" thickBot="1">
+      <c r="B11" s="27"/>
       <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="26"/>
+    <row r="12" spans="2:4" ht="20" thickBot="1">
+      <c r="B12" s="27"/>
       <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="26"/>
+    <row r="13" spans="2:4" ht="20" thickBot="1">
+      <c r="B13" s="27"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="26"/>
+    <row r="14" spans="2:4" ht="20" thickBot="1">
+      <c r="B14" s="27"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="26"/>
+    <row r="15" spans="2:4" ht="20" thickBot="1">
+      <c r="B15" s="27"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="26"/>
+    <row r="16" spans="2:4" ht="20" thickBot="1">
+      <c r="B16" s="27"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="20" t="s">
+    <row r="17" spans="2:4" ht="41" thickBot="1">
+      <c r="B17" s="21" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="4"/>
@@ -1262,20 +1284,20 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="24.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="20"/>
+    <row r="18" spans="2:4" ht="24.75" customHeight="1" thickBot="1">
+      <c r="B18" s="21"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="49.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="20"/>
+    <row r="19" spans="2:4" ht="49.25" customHeight="1" thickBot="1">
+      <c r="B19" s="21"/>
       <c r="C19" s="6"/>
       <c r="D19" s="11"/>
     </row>
-    <row r="20" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="20" t="s">
+    <row r="20" spans="2:4" ht="41" thickBot="1">
+      <c r="B20" s="21" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="4"/>
@@ -1283,15 +1305,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="20"/>
+    <row r="21" spans="2:4" ht="20" thickBot="1">
+      <c r="B21" s="21"/>
       <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="20"/>
+    <row r="22" spans="2:4" ht="20" thickBot="1">
+      <c r="B22" s="21"/>
       <c r="C22" s="6"/>
       <c r="D22" s="11"/>
     </row>
@@ -1313,11 +1335,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054B29E9-D1D3-435F-ADF1-FE65B0763CC2}">
   <dimension ref="B1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
@@ -1325,45 +1347,45 @@
     <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:4" ht="17" thickBot="1"/>
+    <row r="2" spans="2:4" ht="20" thickBot="1">
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="22"/>
-    </row>
-    <row r="3" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="2:4" ht="20" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="22"/>
-    </row>
-    <row r="4" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="2:4" ht="20" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="22"/>
-    </row>
-    <row r="5" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="24"/>
-    </row>
-    <row r="6" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="27" t="s">
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1">
+      <c r="B6" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -1373,83 +1395,83 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="28"/>
+    <row r="7" spans="2:4" ht="41" thickBot="1">
+      <c r="B7" s="29"/>
       <c r="C7" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="28"/>
+    <row r="8" spans="2:4" ht="20" thickBot="1">
+      <c r="B8" s="29"/>
       <c r="C8" s="16"/>
       <c r="D8" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="28"/>
+    <row r="9" spans="2:4" ht="20" thickBot="1">
+      <c r="B9" s="29"/>
       <c r="C9" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="28"/>
+    <row r="10" spans="2:4" ht="41" thickBot="1">
+      <c r="B10" s="29"/>
       <c r="C10" s="16"/>
       <c r="D10" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="28"/>
+    <row r="11" spans="2:4" ht="20" thickBot="1">
+      <c r="B11" s="29"/>
       <c r="C11" s="16"/>
       <c r="D11" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="28"/>
+    <row r="12" spans="2:4" ht="20" thickBot="1">
+      <c r="B12" s="29"/>
       <c r="C12" s="16" t="s">
         <v>44</v>
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="28"/>
+    <row r="13" spans="2:4" ht="20" thickBot="1">
+      <c r="B13" s="29"/>
       <c r="C13" s="16"/>
       <c r="D13" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="28"/>
+    <row r="14" spans="2:4" ht="20" thickBot="1">
+      <c r="B14" s="29"/>
       <c r="C14" s="16"/>
       <c r="D14" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="28"/>
+    <row r="15" spans="2:4" ht="20" thickBot="1">
+      <c r="B15" s="29"/>
       <c r="C15" s="16" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="28"/>
+    <row r="16" spans="2:4" ht="41" thickBot="1">
+      <c r="B16" s="29"/>
       <c r="C16" s="18"/>
       <c r="D16" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="28"/>
+    <row r="17" spans="2:4" ht="20" thickBot="1">
+      <c r="B17" s="29"/>
       <c r="C17" s="17"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="20" t="s">
+    <row r="18" spans="2:4" ht="20" thickBot="1">
+      <c r="B18" s="21" t="s">
         <v>45</v>
       </c>
       <c r="C18" s="5"/>
@@ -1457,13 +1479,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="20"/>
+    <row r="19" spans="2:4" ht="20" thickBot="1">
+      <c r="B19" s="21"/>
       <c r="C19" s="5"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="20"/>
+    <row r="20" spans="2:4" ht="20" thickBot="1">
+      <c r="B20" s="21"/>
       <c r="C20" s="6"/>
       <c r="D20" s="11"/>
     </row>
@@ -1482,13 +1504,126 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B982C2AA-2A13-4FE1-A2EE-7FEF12C78847}">
-  <dimension ref="B1:D17"/>
+  <dimension ref="B1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="37.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="17" thickBot="1"/>
+    <row r="2" spans="2:4" ht="20" thickBot="1">
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="2:4" ht="20" thickBot="1">
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="2:4" ht="20" thickBot="1">
+      <c r="B4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1">
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1">
+      <c r="B6" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="41" thickBot="1">
+      <c r="B7" s="29"/>
+      <c r="C7" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1">
+      <c r="B8" s="29"/>
+      <c r="C8" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" spans="2:4" ht="20" thickBot="1">
+      <c r="B9" s="29"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="20" thickBot="1">
+      <c r="B10" s="29"/>
+      <c r="C10" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="39"/>
+    </row>
+    <row r="11" spans="2:4" ht="61" customHeight="1" thickBot="1">
+      <c r="B11" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:B10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3503E0A-E398-44F1-96F3-85C050C55A58}">
+  <dimension ref="B1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
@@ -1496,45 +1631,45 @@
     <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:4" ht="17" thickBot="1"/>
+    <row r="2" spans="2:4" ht="20" thickBot="1">
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="22"/>
-    </row>
-    <row r="3" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C2" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="2:4" ht="20" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="22"/>
-    </row>
-    <row r="4" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="2:4" ht="20" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="22"/>
-    </row>
-    <row r="5" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="24"/>
-    </row>
-    <row r="6" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="27" t="s">
+      <c r="C5" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="2:4" ht="19" customHeight="1">
+      <c r="B6" s="30" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -1544,66 +1679,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="28"/>
+    <row r="7" spans="2:4" ht="20">
+      <c r="B7" s="31"/>
       <c r="C7" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1">
+      <c r="B8" s="32"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="28"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="28"/>
-      <c r="C9" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="28"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="28"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="28"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="28"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="28"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="28"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="28"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="13"/>
-    </row>
-    <row r="17" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="28"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="3"/>
+    </row>
+    <row r="9" spans="2:4" ht="19">
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="2:4" ht="19">
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+    </row>
+    <row r="11" spans="2:4" ht="19">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1611,173 +1710,126 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B17"/>
+    <mergeCell ref="B6:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3503E0A-E398-44F1-96F3-85C050C55A58}">
-  <dimension ref="B1:D20"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA5DA9D-E6AD-8F4D-93FB-61A3DFB8793B}">
+  <dimension ref="C2:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" customWidth="1"/>
-    <col min="4" max="4" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="38.5" customWidth="1"/>
+    <col min="5" max="5" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="3:5" ht="17" thickBot="1"/>
+    <row r="3" spans="3:5" ht="20" thickBot="1">
+      <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="D3" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="22"/>
-    </row>
-    <row r="3" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="7" t="s">
+      <c r="E3" s="23"/>
+    </row>
+    <row r="4" spans="3:5" ht="20" thickBot="1">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="D4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="22"/>
-    </row>
-    <row r="4" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="7" t="s">
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="3:5" ht="20" thickBot="1">
+      <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="D5" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="22"/>
-    </row>
-    <row r="5" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="7" t="s">
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" spans="3:5" ht="20" thickBot="1">
+      <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="D6" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="3:5" ht="19">
+      <c r="C7" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="20">
+      <c r="C8" s="31"/>
+      <c r="D8" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="24"/>
-    </row>
-    <row r="6" spans="2:4" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="37" x14ac:dyDescent="0.45">
-      <c r="B7" s="30"/>
-      <c r="C7" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="31"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="3:5" ht="19">
+      <c r="C9" s="31"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="33" t="s">
+    <row r="10" spans="3:5" ht="20">
+      <c r="C10" s="33"/>
+      <c r="D10" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="3:5" ht="19">
+      <c r="C11" s="33"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="78.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="34"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="32"/>
-    </row>
-    <row r="11" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="40"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="1" t="s">
+    <row r="12" spans="3:5" ht="20" thickBot="1">
+      <c r="C12" s="34"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="20" t="s">
+    <row r="13" spans="3:5" ht="112" customHeight="1" thickBot="1">
+      <c r="C13" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="36"/>
+      <c r="E13" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="20"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="20"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="53" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B16" s="36"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="39"/>
-    </row>
-    <row r="17" spans="2:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="37"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="D18" s="38"/>
-    </row>
-    <row r="19" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-    </row>
-    <row r="20" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
+  <mergeCells count="5">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C7:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
maquinas de estado done
</commit_message>
<xml_diff>
--- a/Especificacao/especificacaoUseCases.xlsx
+++ b/Especificacao/especificacaoUseCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diogobraga/Desktop/MyChef/Especificacao/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joao/Desktop/Desktop_iCloud/Universidade/3ºano/2ºsemestre/LI4/MyChef/Especificacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B73DB4-C330-9443-8304-6C32F694F8AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08731CFD-AD26-9E43-AFEE-5E110017B973}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Fazer Autenticação" sheetId="1" r:id="rId1"/>
@@ -746,52 +746,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -816,20 +771,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1164,40 +1164,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="31"/>
+      <c r="D2" s="46"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="48"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="49" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1208,61 +1208,61 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="41" thickBot="1">
-      <c r="B7" s="35"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1">
-      <c r="B8" s="35"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1">
-      <c r="B9" s="35"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1">
-      <c r="B10" s="35"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="20" thickBot="1">
-      <c r="B11" s="35"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1">
-      <c r="B12" s="35"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1">
-      <c r="B13" s="35"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1">
-      <c r="B14" s="35"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1">
-      <c r="B15" s="35"/>
+      <c r="B15" s="50"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1">
-      <c r="B16" s="35"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="2:4" ht="20" thickBot="1">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="44" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="4"/>
@@ -1271,12 +1271,12 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="20" thickBot="1">
-      <c r="B18" s="29"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20" thickBot="1">
-      <c r="B19" s="29"/>
+      <c r="B19" s="44"/>
       <c r="C19" s="6"/>
       <c r="D19" s="11"/>
     </row>
@@ -1314,40 +1314,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="31"/>
+      <c r="D2" s="46"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="48"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="49" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1358,71 +1358,71 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="21" thickBot="1">
-      <c r="B7" s="35"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1">
-      <c r="B8" s="35"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1">
-      <c r="B9" s="35"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1">
-      <c r="B10" s="35"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="20" thickBot="1">
-      <c r="B11" s="35"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1">
-      <c r="B12" s="35"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1">
-      <c r="B13" s="35"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1">
-      <c r="B14" s="35"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1">
-      <c r="B15" s="35"/>
+      <c r="B15" s="50"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1">
-      <c r="B16" s="35"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="2:4" ht="41" thickBot="1">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="44" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="4"/>
@@ -1431,19 +1431,19 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="24.75" customHeight="1" thickBot="1">
-      <c r="B18" s="29"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="49.25" customHeight="1" thickBot="1">
-      <c r="B19" s="29"/>
+      <c r="B19" s="44"/>
       <c r="C19" s="6"/>
       <c r="D19" s="11"/>
     </row>
     <row r="20" spans="2:4" ht="41" thickBot="1">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="44" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="4"/>
@@ -1452,14 +1452,14 @@
       </c>
     </row>
     <row r="21" spans="2:4" ht="20" thickBot="1">
-      <c r="B21" s="29"/>
+      <c r="B21" s="44"/>
       <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="20" thickBot="1">
-      <c r="B22" s="29"/>
+      <c r="B22" s="44"/>
       <c r="C22" s="6"/>
       <c r="D22" s="11"/>
     </row>
@@ -1481,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054B29E9-D1D3-435F-ADF1-FE65B0763CC2}">
   <dimension ref="B1:D18"/>
   <sheetViews>
-    <sheetView zoomScale="116" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="116" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -1498,40 +1498,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="31"/>
+      <c r="D2" s="46"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="48"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="52" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -1542,90 +1542,90 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="21" thickBot="1">
-      <c r="B7" s="37"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="15" t="s">
         <v>52</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1">
-      <c r="B8" s="37"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="15"/>
       <c r="D8" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1">
-      <c r="B9" s="37"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="16"/>
       <c r="D9" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1">
-      <c r="B10" s="37"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="16"/>
       <c r="D10" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="41" thickBot="1">
-      <c r="B11" s="37"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="16"/>
       <c r="D11" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1">
-      <c r="B12" s="37"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="16" t="s">
         <v>57</v>
       </c>
       <c r="D12" s="13"/>
     </row>
     <row r="13" spans="2:4" ht="21" thickBot="1">
-      <c r="B13" s="37"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="16"/>
       <c r="D13" s="13" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="24" customHeight="1" thickBot="1">
-      <c r="B14" s="55"/>
-      <c r="C14" s="41"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="77" customHeight="1" thickBot="1">
-      <c r="B15" s="34" t="s">
+    <row r="15" spans="2:4" ht="54" customHeight="1" thickBot="1">
+      <c r="B15" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57" t="s">
+      <c r="C15" s="40"/>
+      <c r="D15" s="41" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="27" customHeight="1" thickBot="1">
-      <c r="B16" s="37"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="58" t="s">
+      <c r="B16" s="51"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="42" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="74" customHeight="1" thickBot="1">
-      <c r="B17" s="34" t="s">
+    <row r="17" spans="2:4" ht="56" customHeight="1" thickBot="1">
+      <c r="B17" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="57" t="s">
+      <c r="C17" s="40"/>
+      <c r="D17" s="41" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26" customHeight="1" thickBot="1">
-      <c r="B18" s="37"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="59" t="s">
+      <c r="B18" s="51"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="43" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1647,7 +1647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C889BB0-E193-2547-94EB-0FEE1062AE77}">
   <dimension ref="B1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="113" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1665,40 +1665,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="31"/>
+      <c r="D2" s="46"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="48"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="52" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -1709,108 +1709,108 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="25" customHeight="1" thickBot="1">
-      <c r="B7" s="36"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46" t="s">
+      <c r="B7" s="52"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="31" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="23" customHeight="1" thickBot="1">
-      <c r="B8" s="37"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="15"/>
       <c r="D8" s="13" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="26" customHeight="1" thickBot="1">
-      <c r="B9" s="37"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="15"/>
       <c r="D9" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="24" customHeight="1" thickBot="1">
-      <c r="B10" s="37"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="15"/>
       <c r="D10" s="13" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="26" customHeight="1" thickBot="1">
-      <c r="B11" s="37"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="15"/>
       <c r="D11" s="13" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="24" customHeight="1" thickBot="1">
-      <c r="B12" s="37"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="15"/>
       <c r="D12" s="13" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="24" customHeight="1" thickBot="1">
-      <c r="B13" s="37"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="15" t="s">
         <v>69</v>
       </c>
       <c r="D13" s="13"/>
     </row>
     <row r="14" spans="2:4" ht="24" customHeight="1" thickBot="1">
-      <c r="B14" s="37"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="54" t="s">
+      <c r="B14" s="51"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="39" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="27" customHeight="1" thickBot="1">
-      <c r="B15" s="37"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="53" t="s">
+      <c r="B15" s="51"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="38" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="23" customHeight="1">
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="49"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="23" customHeight="1">
-      <c r="B17" s="42"/>
-      <c r="C17" s="50"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="26" customHeight="1" thickBot="1">
-      <c r="B18" s="43"/>
-      <c r="C18" s="51"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="36"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="2:4" ht="24" customHeight="1">
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="48" t="s">
+      <c r="C19" s="34"/>
+      <c r="D19" s="33" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="27" customHeight="1">
-      <c r="B20" s="42"/>
-      <c r="C20" s="50"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="20" thickBot="1">
-      <c r="B21" s="43"/>
-      <c r="C21" s="51"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="3"/>
     </row>
   </sheetData>
@@ -1848,40 +1848,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="31"/>
+      <c r="D2" s="46"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="48"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="52" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -1892,28 +1892,28 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="41" thickBot="1">
-      <c r="B7" s="37"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="15" t="s">
         <v>48</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1">
-      <c r="B8" s="37"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="16" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="13"/>
     </row>
     <row r="9" spans="2:4" ht="20" thickBot="1">
-      <c r="B9" s="37"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="16"/>
       <c r="D9" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1">
-      <c r="B10" s="37"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="24" t="s">
         <v>53</v>
       </c>
@@ -1961,40 +1961,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="31"/>
+      <c r="D2" s="46"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="48"/>
     </row>
     <row r="6" spans="2:4" ht="19" customHeight="1">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="57" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -2005,14 +2005,14 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="20">
-      <c r="B7" s="39"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1">
-      <c r="B8" s="40"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="21"/>
       <c r="D8" s="11" t="s">
         <v>37</v>
@@ -2061,40 +2061,40 @@
       <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="31"/>
+      <c r="E3" s="46"/>
     </row>
     <row r="4" spans="3:5" ht="20" thickBot="1">
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="46"/>
     </row>
     <row r="5" spans="3:5" ht="20" thickBot="1">
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="46"/>
     </row>
     <row r="6" spans="3:5" ht="20" thickBot="1">
       <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="33"/>
+      <c r="E6" s="48"/>
     </row>
     <row r="7" spans="3:5" ht="19">
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="57" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="14" t="s">
@@ -2105,14 +2105,14 @@
       </c>
     </row>
     <row r="8" spans="3:5" ht="20">
-      <c r="C8" s="39"/>
+      <c r="C8" s="58"/>
       <c r="D8" s="15" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="3:5" ht="19">
-      <c r="C9" s="39"/>
+      <c r="C9" s="58"/>
       <c r="D9" s="15"/>
       <c r="E9" s="1" t="s">
         <v>42</v>

</xml_diff>